<commit_message>
fourth and seventh form fully reviewed.
</commit_message>
<xml_diff>
--- a/Formatos Finales/formularioSéptimoLleno_1.xlsx
+++ b/Formatos Finales/formularioSéptimoLleno_1.xlsx
@@ -1869,9 +1869,7 @@
       <c r="AL8" s="162" t="n"/>
       <c r="AM8" s="162" t="n"/>
       <c r="AN8" s="163" t="n"/>
-      <c r="AO8" s="40" t="n">
-        <v/>
-      </c>
+      <c r="AO8" s="40" t="n"/>
       <c r="AP8" s="162" t="n"/>
       <c r="AQ8" s="162" t="n"/>
       <c r="AR8" s="162" t="n"/>
@@ -2076,11 +2074,7 @@
         </is>
       </c>
       <c r="S12" s="165" t="n"/>
-      <c r="T12" s="15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="T12" s="15" t="n"/>
       <c r="U12" s="172" t="n"/>
       <c r="AA12" s="165" t="n"/>
       <c r="AB12" s="43" t="n"/>
@@ -2089,17 +2083,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="AM12" s="40" t="n"/>
+      <c r="AM12" s="40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AN12" s="157" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="AO12" s="40" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AO12" s="40" t="n"/>
       <c r="AP12" s="172" t="n"/>
       <c r="AY12" s="165" t="n"/>
     </row>
@@ -2110,7 +2104,11 @@
         </is>
       </c>
       <c r="S13" s="165" t="n"/>
-      <c r="T13" s="15" t="n"/>
+      <c r="T13" s="15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="U13" s="172" t="n"/>
       <c r="AA13" s="165" t="n"/>
       <c r="AB13" s="85" t="inlineStr">
@@ -2204,7 +2202,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AO15" s="40" t="n"/>
+      <c r="AO15" s="40" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AP15" s="172" t="n"/>
       <c r="AY15" s="165" t="n"/>
     </row>
@@ -2215,18 +2217,18 @@
         </is>
       </c>
       <c r="E16" s="165" t="n"/>
-      <c r="F16" s="15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="F16" s="15" t="n"/>
       <c r="G16" s="174" t="inlineStr">
         <is>
           <t>Cooperativa</t>
         </is>
       </c>
       <c r="L16" s="165" t="n"/>
-      <c r="M16" s="15" t="n"/>
+      <c r="M16" s="15" t="inlineStr">
+        <is>
+          <t>Cooperativa</t>
+        </is>
+      </c>
       <c r="N16" s="175" t="inlineStr">
         <is>
           <t>Otro ¿Cuál?</t>
@@ -2238,8 +2240,10 @@
           <t xml:space="preserve">Observaciones: </t>
         </is>
       </c>
-      <c r="AI16" s="56" t="n">
-        <v/>
+      <c r="AI16" s="56" t="inlineStr">
+        <is>
+          <t>sfg</t>
+        </is>
       </c>
       <c r="AJ16" s="167" t="n"/>
       <c r="AK16" s="167" t="n"/>
@@ -2387,17 +2391,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="L19" s="15" t="n"/>
+      <c r="L19" s="15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="M19" s="3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="N19" s="40" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="N19" s="40" t="n"/>
       <c r="O19" s="163" t="n"/>
       <c r="P19" s="79" t="inlineStr">
         <is>
@@ -2430,17 +2434,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="AS19" s="15" t="n"/>
+      <c r="AS19" s="15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AT19" s="157" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="AU19" s="15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AU19" s="15" t="n"/>
       <c r="AV19" s="172" t="n"/>
       <c r="AY19" s="165" t="n"/>
     </row>
@@ -2497,17 +2501,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="AS20" s="15" t="inlineStr">
+      <c r="AS20" s="15" t="n"/>
+      <c r="AT20" s="157" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU20" s="15" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="AT20" s="157" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="AU20" s="15" t="n"/>
       <c r="AV20" s="178" t="n"/>
       <c r="AW20" s="167" t="n"/>
       <c r="AX20" s="167" t="n"/>
@@ -2666,17 +2670,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="H24" s="15" t="inlineStr">
+      <c r="H24" s="15" t="n"/>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="J24" s="15" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="I24" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="J24" s="15" t="n"/>
       <c r="K24" s="172" t="n"/>
       <c r="AA24" s="165" t="n"/>
       <c r="AB24" s="181" t="inlineStr">
@@ -2715,11 +2719,7 @@
           <t xml:space="preserve">¿Cuál? </t>
         </is>
       </c>
-      <c r="D25" s="55" t="inlineStr">
-        <is>
-          <t>Transportes LTDA</t>
-        </is>
-      </c>
+      <c r="D25" s="55" t="n"/>
       <c r="E25" s="167" t="n"/>
       <c r="F25" s="167" t="n"/>
       <c r="G25" s="167" t="n"/>
@@ -2732,9 +2732,7 @@
           <t>Número de contacto</t>
         </is>
       </c>
-      <c r="R25" s="56" t="n">
-        <v>555555555</v>
-      </c>
+      <c r="R25" s="56" t="n"/>
       <c r="S25" s="167" t="n"/>
       <c r="T25" s="167" t="n"/>
       <c r="U25" s="167" t="n"/>
@@ -2823,11 +2821,7 @@
         </is>
       </c>
       <c r="AR27" s="165" t="n"/>
-      <c r="AS27" s="15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AS27" s="15" t="n"/>
       <c r="AT27" s="173" t="n"/>
       <c r="AY27" s="165" t="n"/>
     </row>
@@ -2895,7 +2889,11 @@
         </is>
       </c>
       <c r="AR29" s="165" t="n"/>
-      <c r="AS29" s="15" t="n"/>
+      <c r="AS29" s="15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AT29" s="173" t="n"/>
       <c r="AY29" s="165" t="n"/>
     </row>
@@ -2957,9 +2955,7 @@
       <c r="AY30" s="168" t="n"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="43" t="n">
-        <v>10</v>
-      </c>
+      <c r="A31" s="43" t="n"/>
       <c r="V31" s="157" t="inlineStr">
         <is>
           <t>%</t>
@@ -3034,17 +3030,17 @@
           <t>Si</t>
         </is>
       </c>
-      <c r="AN32" s="15" t="n"/>
+      <c r="AN32" s="15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="AO32" s="3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="AP32" s="15" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="AP32" s="15" t="n"/>
       <c r="AQ32" s="172" t="n"/>
       <c r="AY32" s="165" t="n"/>
     </row>
@@ -3089,7 +3085,7 @@
         </is>
       </c>
       <c r="AL33" s="55" t="n">
-        <v/>
+        <v>3635</v>
       </c>
       <c r="AM33" s="167" t="n"/>
       <c r="AN33" s="167" t="n"/>
@@ -3247,9 +3243,7 @@
     </row>
     <row r="37">
       <c r="A37" s="43" t="n"/>
-      <c r="C37" s="55" t="n">
-        <v>5</v>
-      </c>
+      <c r="C37" s="55" t="n"/>
       <c r="D37" s="167" t="n"/>
       <c r="E37" s="167" t="n"/>
       <c r="F37" s="167" t="n"/>

</xml_diff>